<commit_message>
Change deadband cases to PVD2 and ESD2
</commit_message>
<xml_diff>
--- a/demo/deadband/cases/IL200_opf2.xlsx
+++ b/demo/deadband/cases/IL200_opf2.xlsx
@@ -15,13 +15,14 @@
     <sheet name="Line" sheetId="6" r:id="rId6"/>
     <sheet name="Area" sheetId="7" r:id="rId7"/>
     <sheet name="GCost" sheetId="8" r:id="rId8"/>
+    <sheet name="Summary" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="702">
   <si>
     <t>idx</t>
   </si>
@@ -2100,6 +2101,33 @@
   </si>
   <si>
     <t>c0</t>
+  </si>
+  <si>
+    <t>field</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>comment2</t>
+  </si>
+  <si>
+    <t>comment3</t>
+  </si>
+  <si>
+    <t>comment4</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>AMS 1.0.12.post44+g71e1785f</t>
+  </si>
+  <si>
+    <t>06/04/2025 10:34:39 PM</t>
+  </si>
+  <si>
+    <t>AMS comes with ABSOLUTELY NO WARRANTY</t>
   </si>
 </sst>
 </file>
@@ -45395,4 +45423,54 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>698</v>
+      </c>
+      <c r="C2" t="s">
+        <v>699</v>
+      </c>
+      <c r="D2" t="s">
+        <v>700</v>
+      </c>
+      <c r="E2" t="s">
+        <v>701</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Minor fix in deadband case
</commit_message>
<xml_diff>
--- a/demo/deadband/cases/IL200_opf2.xlsx
+++ b/demo/deadband/cases/IL200_opf2.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="702">
   <si>
     <t>idx</t>
   </si>
@@ -2121,10 +2121,10 @@
     <t>Info</t>
   </si>
   <si>
-    <t>AMS 1.0.12.post44+g71e1785f</t>
-  </si>
-  <si>
-    <t>06/04/2025 10:34:39 PM</t>
+    <t>AMS 1.0.12.post44.dev0+g71e1785f</t>
+  </si>
+  <si>
+    <t>06/05/2025 06:07:12 PM</t>
   </si>
   <si>
     <t>AMS comes with ABSOLUTELY NO WARRANTY</t>
@@ -45437,6 +45437,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>693</v>
       </c>

</xml_diff>